<commit_message>
Added neutral to classes
</commit_message>
<xml_diff>
--- a/training data/categories/datacategories.xlsx
+++ b/training data/categories/datacategories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clinvil/Programs/ToneAI/training data/categories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D34C5C7-35BD-9348-9376-16C562879BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2EA4C7-CE0F-2248-B1BD-C8E454381911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440" xr2:uid="{C67D7A24-B123-3245-A23A-008792837BF4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Id</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>I3</t>
+  </si>
+  <si>
+    <t>Neutral</t>
   </si>
 </sst>
 </file>
@@ -462,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86C1DA4-0E1E-C74D-BD88-D1E79109599A}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,36 +481,39 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>